<commit_message>
Add initial report and additional plots in repo
</commit_message>
<xml_diff>
--- a/FarePredictor/model_dev/delivered/model_performance.xlsx
+++ b/FarePredictor/model_dev/delivered/model_performance.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josuero.cuevasjuarez/Desktop/Desktop/take_home_assignment/model_dev/delivered/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josue\Desktop\ownrepos\FarePredictor\model_dev\delivered\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD94C5BA-5291-E749-8C3E-9A430DCDC894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21220" yWindow="2880" windowWidth="28240" windowHeight="17440" xr2:uid="{8FAFC16C-6D7A-D946-A331-A1710C2053C4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Final_model" sheetId="1" r:id="rId1"/>
@@ -56,22 +55,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00000000_ "/>
+    <numFmt numFmtId="164" formatCode="0.00000000_ "/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -129,16 +128,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -454,29 +453,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0AB94C40-7054-A745-A24B-586F17AF84B2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1"/>
-    <col min="2" max="2" width="21.140625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" width="10.75" style="1"/>
+    <col min="2" max="2" width="21.125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="32" customHeight="1">
+    <row r="1" spans="1:2" ht="32.1" customHeight="1">
       <c r="B1" s="4"/>
     </row>
-    <row r="2" spans="1:2" ht="17">
+    <row r="2" spans="1:2">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="17">
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -484,7 +483,7 @@
         <v>0.97123309068990205</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="17">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -492,7 +491,7 @@
         <v>5.4748955859155197</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="17">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>

</xml_diff>